<commit_message>
students work. university left
</commit_message>
<xml_diff>
--- a/info_02/src/main/resources/universityInfo.xlsx
+++ b/info_02/src/main/resources/universityInfo.xlsx
@@ -8,13 +8,15 @@
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="Студенты" sheetId="2" r:id="rId5"/>
     <sheet name="Университеты" sheetId="3" r:id="rId6"/>
-    <sheet name="Лист3" sheetId="4" r:id="rId7"/>
+    <sheet name="Студенты-1" sheetId="4" r:id="rId7"/>
+    <sheet name="Университеты-1" sheetId="5" r:id="rId8"/>
+    <sheet name="Лист3" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -28,10 +30,163 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Студенты</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Студенты</t>
+    </r>
+  </si>
+  <si>
+    <t>Университеты</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Университеты</t>
+    </r>
+  </si>
+  <si>
+    <t>Лист3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Лист3</t>
+    </r>
+  </si>
+  <si>
+    <t>0002-high</t>
+  </si>
+  <si>
+    <t>Иванов И. А.</t>
+  </si>
+  <si>
+    <t>Козлов М. В.</t>
+  </si>
+  <si>
+    <t>Фёдоров А. И.</t>
+  </si>
+  <si>
+    <t>0003-high</t>
+  </si>
+  <si>
+    <t>Игнатьев М. М.</t>
+  </si>
+  <si>
+    <t>0004-high</t>
+  </si>
+  <si>
+    <t>Соколов В. В.</t>
+  </si>
+  <si>
+    <t>Сидоров Е. Г.</t>
+  </si>
+  <si>
+    <t>0001-high</t>
+  </si>
+  <si>
+    <t>Витальев В. А.</t>
+  </si>
+  <si>
+    <t>Петров П. А.</t>
+  </si>
+  <si>
+    <t>Алексеев С. В.</t>
+  </si>
+  <si>
+    <t>Иванов А. Г.</t>
+  </si>
+  <si>
+    <t>Васильев В. П.</t>
+  </si>
+  <si>
+    <t>Московский Выдуманный Университет</t>
+  </si>
+  <si>
+    <t>МВУ</t>
+  </si>
+  <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t>Московский Придуманный Институт</t>
+  </si>
+  <si>
+    <t>МПИ</t>
+  </si>
+  <si>
+    <t>Московский Государственный Медицинский Университет</t>
+  </si>
+  <si>
+    <t>МГМУ</t>
+  </si>
+  <si>
+    <t>MEDICINE</t>
+  </si>
+  <si>
+    <t>Тамбовский Университет Медицины</t>
+  </si>
+  <si>
+    <t>ТУМ</t>
+  </si>
+  <si>
+    <t>0005-high</t>
+  </si>
+  <si>
+    <t>Самарский Медицинский Институт</t>
+  </si>
+  <si>
+    <t>СМИ</t>
+  </si>
+  <si>
+    <t>0006-high</t>
+  </si>
+  <si>
+    <t>Воронежский Литературно-Переводческий Университет</t>
+  </si>
+  <si>
+    <t>ВЛПУ</t>
+  </si>
+  <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t>0007-high</t>
+  </si>
+  <si>
+    <t>Казанский Университет Вычислений</t>
+  </si>
+  <si>
+    <t>КУВ</t>
+  </si>
+  <si>
+    <t>MATHEMATICS</t>
+  </si>
+  <si>
+    <t>Студенты-1</t>
   </si>
   <si>
     <t>id университета</t>
@@ -46,52 +201,7 @@
     <t>Средний балл</t>
   </si>
   <si>
-    <t>0002-high</t>
-  </si>
-  <si>
-    <t>Иванов И. А.</t>
-  </si>
-  <si>
-    <t>Козлов М. В.</t>
-  </si>
-  <si>
-    <t>Фёдоров А. И.</t>
-  </si>
-  <si>
-    <t>0003-high</t>
-  </si>
-  <si>
-    <t>Игнатьев М. М.</t>
-  </si>
-  <si>
-    <t>0004-high</t>
-  </si>
-  <si>
-    <t>Соколов В. В.</t>
-  </si>
-  <si>
-    <t>Сидоров Е. Г.</t>
-  </si>
-  <si>
-    <t>0001-high</t>
-  </si>
-  <si>
-    <t>Витальев В. А.</t>
-  </si>
-  <si>
-    <t>Петров П. А.</t>
-  </si>
-  <si>
-    <t>Алексеев С. В.</t>
-  </si>
-  <si>
-    <t>Иванов А. Г.</t>
-  </si>
-  <si>
-    <t>Васильев В. П.</t>
-  </si>
-  <si>
-    <t>Университеты</t>
+    <t>Университеты-1</t>
   </si>
   <si>
     <t>Полное название</t>
@@ -104,72 +214,6 @@
   </si>
   <si>
     <t>Профиль обучения</t>
-  </si>
-  <si>
-    <t>Московский Выдуманный Университет</t>
-  </si>
-  <si>
-    <t>МВУ</t>
-  </si>
-  <si>
-    <t>PHYSICS</t>
-  </si>
-  <si>
-    <t>Московский Придуманный Институт</t>
-  </si>
-  <si>
-    <t>МПИ</t>
-  </si>
-  <si>
-    <t>Московский Государственный Медицинский Университет</t>
-  </si>
-  <si>
-    <t>МГМУ</t>
-  </si>
-  <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
-    <t>Тамбовский Университет Медицины</t>
-  </si>
-  <si>
-    <t>ТУМ</t>
-  </si>
-  <si>
-    <t>0005-high</t>
-  </si>
-  <si>
-    <t>Самарский Медицинский Институт</t>
-  </si>
-  <si>
-    <t>СМИ</t>
-  </si>
-  <si>
-    <t>0006-high</t>
-  </si>
-  <si>
-    <t>Воронежский Литературно-Переводческий Университет</t>
-  </si>
-  <si>
-    <t>ВЛПУ</t>
-  </si>
-  <si>
-    <t>LINGUISTICS</t>
-  </si>
-  <si>
-    <t>0007-high</t>
-  </si>
-  <si>
-    <t>Казанский Университет Вычислений</t>
-  </si>
-  <si>
-    <t>КУВ</t>
-  </si>
-  <si>
-    <t>MATHEMATICS</t>
-  </si>
-  <si>
-    <t>Лист3</t>
   </si>
 </sst>
 </file>
@@ -218,7 +262,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,8 +281,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -248,16 +298,103 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -267,7 +404,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -289,19 +426,82 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -330,6 +530,7 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -481,9 +682,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -563,7 +764,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -591,10 +792,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -850,9 +1051,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1140,7 +1341,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1168,10 +1369,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1422,284 +1623,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>51</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" ht="13" customHeight="1">
+      <c r="A15" s="7"/>
+      <c r="B15" t="s" s="3">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" ht="13" customHeight="1">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4"/>
+      <c r="C16" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>48</v>
+      </c>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Студенты'!R1C1" tooltip="" display="Студенты"/>
-    <hyperlink ref="D12" location="'Университеты'!R1C1" tooltip="" display="Университеты"/>
-    <hyperlink ref="D14" location="'Лист3'!R1C1" tooltip="" display="Лист3"/>
+    <hyperlink ref="D12" location="'Студенты'!R1C1" tooltip="" display="Студенты"/>
+    <hyperlink ref="D14" location="'Университеты'!R1C1" tooltip="" display="Университеты"/>
+    <hyperlink ref="D16" location="'Лист3'!R1C1" tooltip="" display="Лист3"/>
+    <hyperlink ref="D12" location="'Студенты'!R1C1" tooltip="" display="Студенты"/>
+    <hyperlink ref="D14" location="'Университеты'!R1C1" tooltip="" display="Университеты"/>
+    <hyperlink ref="D16" location="'Студенты-1'!R1C1" tooltip="" display="Студенты-1"/>
+    <hyperlink ref="D18" location="'Университеты-1'!R1C1" tooltip="" display="Университеты-1"/>
+    <hyperlink ref="D20" location="'Лист3'!R1C1" tooltip="" display="Лист3"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="12.8516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="25" customWidth="1"/>
+    <col min="4" max="4" width="12.1719" style="25" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="E1" s="8"/>
+      <c r="A1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="C1" s="27">
+        <v>2</v>
+      </c>
+      <c r="D1" s="28">
+        <v>4</v>
+      </c>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C2" s="10">
+      <c r="A2" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>14</v>
+      </c>
+      <c r="C2" s="27">
         <v>2</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="28">
+        <v>4.6</v>
+      </c>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="28">
+        <v>4.2</v>
+      </c>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C4" s="27">
         <v>4</v>
       </c>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="9">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="D4" s="28">
+        <v>4.3</v>
+      </c>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="C5" s="27">
         <v>2</v>
       </c>
-      <c r="D3" s="11">
-        <v>4.6</v>
-      </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="D5" s="28">
+        <v>4.8</v>
+      </c>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="C6" s="27">
         <v>3</v>
       </c>
-      <c r="D4" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="D6" s="28">
+        <v>3.9</v>
+      </c>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s" s="26">
+        <v>22</v>
+      </c>
+      <c r="C7" s="27">
+        <v>1</v>
+      </c>
+      <c r="D7" s="28">
         <v>4</v>
       </c>
-      <c r="D5" s="11">
-        <v>4.3</v>
-      </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="C8" s="27">
         <v>1</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D8" s="28">
+        <v>5</v>
+      </c>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="26">
+        <v>24</v>
+      </c>
+      <c r="C9" s="27">
+        <v>2</v>
+      </c>
+      <c r="D9" s="28">
+        <v>5</v>
+      </c>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="26">
+        <v>25</v>
+      </c>
+      <c r="C10" s="27">
+        <v>3</v>
+      </c>
+      <c r="D10" s="28">
         <v>4.8</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11">
-        <v>3.9</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10">
-        <v>2</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="26">
+        <v>26</v>
+      </c>
+      <c r="C11" s="27">
         <v>4</v>
       </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C10" s="10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="C11" s="10">
-        <v>3</v>
-      </c>
-      <c r="D11" s="11">
-        <v>4.8</v>
-      </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="C12" s="10">
-        <v>4</v>
-      </c>
-      <c r="D12" s="11">
+      <c r="D11" s="28">
         <v>4.7</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E11" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,180 +2035,162 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="15.6719" style="12" customWidth="1"/>
-    <col min="2" max="2" width="55" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.1719" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.6719" style="12" customWidth="1"/>
-    <col min="6" max="6" width="8.85156" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="15.6719" style="30" customWidth="1"/>
+    <col min="2" max="2" width="45.8516" style="30" customWidth="1"/>
+    <col min="3" max="3" width="14.1719" style="30" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="30" customWidth="1"/>
+    <col min="5" max="5" width="16.1719" style="30" customWidth="1"/>
+    <col min="6" max="6" width="8.85156" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s" s="7">
+      <c r="A1" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s" s="26">
         <v>27</v>
       </c>
-      <c r="D1" t="s" s="7">
+      <c r="C1" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="E1" t="s" s="7">
+      <c r="D1" s="27">
+        <v>1980</v>
+      </c>
+      <c r="E1" t="s" s="26">
         <v>29</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s" s="9">
+      <c r="A2" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="26">
         <v>30</v>
       </c>
-      <c r="C2" t="s" s="9">
+      <c r="C2" t="s" s="26">
         <v>31</v>
       </c>
-      <c r="D2" s="10">
-        <v>1990</v>
-      </c>
-      <c r="E2" t="s" s="9">
+      <c r="D2" s="27">
+        <v>1988</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="26">
         <v>32</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="9">
+      <c r="C3" t="s" s="26">
         <v>33</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="D3" s="27">
+        <v>1977</v>
+      </c>
+      <c r="E3" t="s" s="26">
         <v>34</v>
       </c>
-      <c r="D3" s="10">
-        <v>1987</v>
-      </c>
-      <c r="E3" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="9">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="9">
+      <c r="A4" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="26">
         <v>35</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="26">
         <v>36</v>
       </c>
-      <c r="D4" s="10">
-        <v>1960</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="D4" s="27">
+        <v>1999</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="26">
         <v>37</v>
       </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s" s="9">
+      <c r="B5" t="s" s="26">
         <v>38</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" t="s" s="26">
         <v>39</v>
       </c>
-      <c r="D5" s="10">
-        <v>1995</v>
-      </c>
-      <c r="E5" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="D5" s="27">
+        <v>1999</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="F5" s="29"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="9">
+      <c r="A6" t="s" s="26">
         <v>40</v>
       </c>
-      <c r="B6" t="s" s="9">
+      <c r="B6" t="s" s="26">
         <v>41</v>
       </c>
-      <c r="C6" t="s" s="9">
+      <c r="C6" t="s" s="26">
         <v>42</v>
       </c>
-      <c r="D6" s="10">
-        <v>1936</v>
-      </c>
-      <c r="E6" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="F6" s="8"/>
+      <c r="D6" s="27">
+        <v>1967</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="F6" s="29"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s" s="9">
+      <c r="A7" t="s" s="26">
         <v>44</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="B7" t="s" s="26">
         <v>45</v>
       </c>
-      <c r="D7" s="10">
-        <v>2003</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="C7" t="s" s="26">
         <v>46</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="D7" s="27">
+        <v>1950</v>
+      </c>
+      <c r="E7" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s" s="9">
-        <v>49</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1989</v>
-      </c>
-      <c r="E8" t="s" s="9">
-        <v>50</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1898,85 +2203,476 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="31" customWidth="1"/>
+    <col min="2" max="2" width="12.8516" style="31" customWidth="1"/>
+    <col min="3" max="3" width="8.85156" style="31" customWidth="1"/>
+    <col min="4" max="4" width="12.1719" style="31" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="32">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s" s="32">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="C2" s="27">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28">
+        <v>4</v>
+      </c>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>14</v>
+      </c>
+      <c r="C3" s="27">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28">
+        <v>4.6</v>
+      </c>
+      <c r="E3" s="29"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>15</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="28">
+        <v>4.2</v>
+      </c>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>17</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="28">
+        <v>4.3</v>
+      </c>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="C6" s="27">
+        <v>2</v>
+      </c>
+      <c r="D6" s="28">
+        <v>4.8</v>
+      </c>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s" s="26">
+        <v>20</v>
+      </c>
+      <c r="C7" s="27">
+        <v>3</v>
+      </c>
+      <c r="D7" s="28">
+        <v>3.9</v>
+      </c>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s" s="26">
+        <v>22</v>
+      </c>
+      <c r="C8" s="27">
+        <v>1</v>
+      </c>
+      <c r="D8" s="28">
+        <v>4</v>
+      </c>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="C9" s="27">
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
+        <v>5</v>
+      </c>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="26">
+        <v>24</v>
+      </c>
+      <c r="C10" s="27">
+        <v>2</v>
+      </c>
+      <c r="D10" s="28">
+        <v>5</v>
+      </c>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="26">
+        <v>25</v>
+      </c>
+      <c r="C11" s="27">
+        <v>3</v>
+      </c>
+      <c r="D11" s="28">
+        <v>4.8</v>
+      </c>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="26">
+        <v>26</v>
+      </c>
+      <c r="C12" s="27">
+        <v>4</v>
+      </c>
+      <c r="D12" s="28">
+        <v>4.7</v>
+      </c>
+      <c r="E12" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="15.6719" style="33" customWidth="1"/>
+    <col min="2" max="2" width="45.8516" style="33" customWidth="1"/>
+    <col min="3" max="3" width="14.1719" style="33" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="33" customWidth="1"/>
+    <col min="5" max="5" width="16.1719" style="33" customWidth="1"/>
+    <col min="6" max="6" width="8.85156" style="33" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="32">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s" s="32">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s" s="32">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s" s="32">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s" s="32">
+        <v>57</v>
+      </c>
+      <c r="F1" s="29"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="26">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="26">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s" s="26">
+        <v>28</v>
+      </c>
+      <c r="D2" s="27">
+        <v>1980</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="26">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s" s="26">
+        <v>31</v>
+      </c>
+      <c r="D3" s="27">
+        <v>1988</v>
+      </c>
+      <c r="E3" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="26">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s" s="26">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="D4" s="27">
+        <v>1977</v>
+      </c>
+      <c r="E4" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="26">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="26">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s" s="26">
+        <v>36</v>
+      </c>
+      <c r="D5" s="27">
+        <v>1999</v>
+      </c>
+      <c r="E5" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="F5" s="29"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="26">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s" s="26">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s" s="26">
+        <v>39</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1999</v>
+      </c>
+      <c r="E6" t="s" s="26">
+        <v>34</v>
+      </c>
+      <c r="F6" s="29"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="26">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s" s="26">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s" s="26">
+        <v>42</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1967</v>
+      </c>
+      <c r="E7" t="s" s="26">
+        <v>43</v>
+      </c>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="26">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s" s="26">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s" s="26">
+        <v>46</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1950</v>
+      </c>
+      <c r="E8" t="s" s="26">
+        <v>47</v>
+      </c>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="13" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>